<commit_message>
Added Problem 2 Description
</commit_message>
<xml_diff>
--- a/DS_Algo_Code_Book.xlsx
+++ b/DS_Algo_Code_Book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebinmathew/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebinmathew/Desktop/Sebin Mathew/Tech Resources/DSAlgo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6BE9ED4-4B7B-EC4E-8B4E-8FB16E7F2412}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BCD65A-E19D-294B-99B6-CF4F9820FDDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D556291A-005B-4940-9EC0-89385B5AB12F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D556291A-005B-4940-9EC0-89385B5AB12F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Sl. No</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Sum of elements equal to target in an array.</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -69,6 +66,19 @@
   </si>
   <si>
     <t xml:space="preserve">O(n). Two iterations. Extra space fof hashmap. </t>
+  </si>
+  <si>
+    <t>Sum of elements equal to target in an array.  
+Modification : No duplicates, only unique pairs</t>
+  </si>
+  <si>
+    <t>Print element and number of repetitions with the least extra space. Numbers will be repeated in a group and not randomly placed. Every number repeats atleast twice. 
+Ex : 2 2 3 3 3 3 4 4 5 5 5 -&gt; input 2 2 3 4 4 2 5 3 -&gt; output
+Modification : Number may repeat only once
+Ex : 2 3 3 4 5 5 -&gt; input  2 1 3 2 4 1 5 2 -&gt; output</t>
+  </si>
+  <si>
+    <t>Array manipulation</t>
   </si>
 </sst>
 </file>
@@ -104,17 +114,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,13 +446,14 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.83203125" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
@@ -457,61 +471,75 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2"/>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="4"/>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>38718</v>
+      </c>
+      <c r="H3" s="2">
+        <v>38718</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3">
-        <v>38718</v>
-      </c>
-      <c r="H3" s="3">
-        <v>38718</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:9" ht="110" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>39083</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added GCD and Nth Node from end
</commit_message>
<xml_diff>
--- a/DS_Algo_Code_Book.xlsx
+++ b/DS_Algo_Code_Book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebinmathew/Desktop/Sebin Mathew/Tech Resources/DSAlgo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A840C2F6-FD1D-B047-ACA7-2DBC373135BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6EF81A-7E6B-EB4A-BB5C-9D5563C8269F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D556291A-005B-4940-9EC0-89385B5AB12F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Sl. No</t>
   </si>
@@ -111,6 +111,22 @@
   <si>
     <t>Array Rotation by k units to right.
 Modified : k units to left</t>
+  </si>
+  <si>
+    <t>GCD of two numbers
+Note : GCD(a,b) = GCD(b,a)</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Nth Node from end with all corner cases</t>
+  </si>
+  <si>
+    <t>Lists</t>
+  </si>
+  <si>
+    <t>O(n)</t>
   </si>
 </sst>
 </file>
@@ -151,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +181,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD0AB5D-282B-614B-9A84-5AD7EB51735C}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -514,17 +533,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,6 +630,49 @@
       </c>
       <c r="I5" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>38749</v>
+      </c>
+      <c r="H6" s="2">
+        <v>38749</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>38749</v>
+      </c>
+      <c r="H7" s="2">
+        <v>38749</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>